<commit_message>
Sprint 20 End results
</commit_message>
<xml_diff>
--- a/bant_sprint_20.xlsx
+++ b/bant_sprint_20.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="67">
   <si>
     <t>Key</t>
   </si>
@@ -47,150 +47,135 @@
     <t>Project</t>
   </si>
   <si>
-    <t>BANTS-11</t>
+    <t>BANTI-78</t>
+  </si>
+  <si>
+    <t>Bug</t>
+  </si>
+  <si>
+    <t>Unable to create an Insulin reading</t>
+  </si>
+  <si>
+    <t>Closed</t>
+  </si>
+  <si>
+    <t>bant - iOS</t>
+  </si>
+  <si>
+    <t>BANTI-76</t>
+  </si>
+  <si>
+    <t>Feature</t>
+  </si>
+  <si>
+    <t>MealReading Overview View Controller</t>
+  </si>
+  <si>
+    <t>BANTI-75</t>
+  </si>
+  <si>
+    <t>BantBook no longer loads</t>
+  </si>
+  <si>
+    <t>BANTI-62</t>
+  </si>
+  <si>
+    <t>Enhancement</t>
+  </si>
+  <si>
+    <t>Make the settings button easier to click</t>
+  </si>
+  <si>
+    <t>Ready to Merge</t>
+  </si>
+  <si>
+    <t>BANTI-59</t>
   </si>
   <si>
     <t>Chore</t>
   </si>
   <si>
-    <t>Setup email for bant</t>
-  </si>
-  <si>
-    <t>Closed</t>
-  </si>
-  <si>
-    <t>bant - Server</t>
-  </si>
-  <si>
-    <t>BANTI-77</t>
-  </si>
-  <si>
-    <t>Bug</t>
-  </si>
-  <si>
-    <t>Steps algorithm gives incorrect trends</t>
+    <t>Design Meal Model</t>
+  </si>
+  <si>
+    <t>BANTI-56</t>
+  </si>
+  <si>
+    <t>ResetPasswordViewController</t>
+  </si>
+  <si>
+    <t>Review</t>
+  </si>
+  <si>
+    <t>BANTI-55</t>
+  </si>
+  <si>
+    <t>LoginViewController</t>
+  </si>
+  <si>
+    <t>BANTI-54</t>
+  </si>
+  <si>
+    <t>CreateAccountViewController</t>
+  </si>
+  <si>
+    <t>BANTI-53</t>
+  </si>
+  <si>
+    <t>Functional Wireframing</t>
+  </si>
+  <si>
+    <t>BANTI-51</t>
+  </si>
+  <si>
+    <t>Import legacy database components from old Bant code-base</t>
+  </si>
+  <si>
+    <t>BANTI-48</t>
+  </si>
+  <si>
+    <t>Authentication framework controllers</t>
+  </si>
+  <si>
+    <t>BANTI-47</t>
+  </si>
+  <si>
+    <t>Convert from legacy</t>
+  </si>
+  <si>
+    <t>In Progress</t>
+  </si>
+  <si>
+    <t>BANTI-42</t>
+  </si>
+  <si>
+    <t>Categorizing and diagraming required classes and objects</t>
+  </si>
+  <si>
+    <t>BANTA-323</t>
+  </si>
+  <si>
+    <t>Copy Changes in Trends</t>
+  </si>
+  <si>
+    <t>bant - Android</t>
+  </si>
+  <si>
+    <t>BANTA-321</t>
+  </si>
+  <si>
+    <t>Implement Syncing so Far into the App</t>
+  </si>
+  <si>
+    <t>BANTA-320</t>
+  </si>
+  <si>
+    <t>Create Analytics Framework</t>
   </si>
   <si>
     <t>Open</t>
   </si>
   <si>
-    <t>bant - iOS</t>
-  </si>
-  <si>
-    <t>BANTI-76</t>
-  </si>
-  <si>
-    <t>Feature</t>
-  </si>
-  <si>
-    <t>MealReading Overview View Controller</t>
-  </si>
-  <si>
-    <t>Review</t>
-  </si>
-  <si>
-    <t>BANTI-75</t>
-  </si>
-  <si>
-    <t>BantBook no longer loads</t>
-  </si>
-  <si>
-    <t>BANTI-62</t>
-  </si>
-  <si>
-    <t>Enhancement</t>
-  </si>
-  <si>
-    <t>Make the settings button easier to click</t>
-  </si>
-  <si>
-    <t>Ready to Merge</t>
-  </si>
-  <si>
-    <t>BANTI-59</t>
-  </si>
-  <si>
-    <t>Design Meal Model</t>
-  </si>
-  <si>
-    <t>BANTI-56</t>
-  </si>
-  <si>
-    <t>ResetPasswordViewController</t>
-  </si>
-  <si>
-    <t>BANTI-55</t>
-  </si>
-  <si>
-    <t>LoginViewController</t>
-  </si>
-  <si>
-    <t>BANTI-54</t>
-  </si>
-  <si>
-    <t>CreateAccountViewController</t>
-  </si>
-  <si>
-    <t>BANTI-53</t>
-  </si>
-  <si>
-    <t>Functional Wireframing</t>
-  </si>
-  <si>
-    <t>In Progress</t>
-  </si>
-  <si>
-    <t>BANTI-51</t>
-  </si>
-  <si>
-    <t>Import legacy database components from old Bant code-base</t>
-  </si>
-  <si>
-    <t>BANTI-48</t>
-  </si>
-  <si>
-    <t>Authentication framework controllers</t>
-  </si>
-  <si>
-    <t>BANTI-47</t>
-  </si>
-  <si>
-    <t>Convert from legacy</t>
-  </si>
-  <si>
-    <t>BANTI-42</t>
-  </si>
-  <si>
-    <t>Categorizing and diagraming required classes and objects</t>
-  </si>
-  <si>
-    <t>BANTA-323</t>
-  </si>
-  <si>
-    <t>Copy Changes in Trends</t>
-  </si>
-  <si>
-    <t>bant - Android</t>
-  </si>
-  <si>
-    <t>BANTA-322</t>
-  </si>
-  <si>
-    <t>Timeline Planning Conversation</t>
-  </si>
-  <si>
-    <t>BANTA-321</t>
-  </si>
-  <si>
-    <t>Implement Syncing so Far into the App</t>
-  </si>
-  <si>
-    <t>BANTA-320</t>
-  </si>
-  <si>
-    <t>Create Analytics Framework</t>
-  </si>
-  <si>
     <t>BANTA-317</t>
   </si>
   <si>
@@ -213,9 +198,6 @@
   </si>
   <si>
     <t>Target range changes are no longer saved in the preferences menu</t>
-  </si>
-  <si>
-    <t>Testing</t>
   </si>
   <si>
     <t>BANTA-287</t>
@@ -611,10 +593,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -659,7 +641,7 @@
         <v>8</v>
       </c>
       <c r="D2" s="5">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>9</v>
@@ -682,181 +664,181 @@
         <v>2</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D4" s="5">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D5" s="5">
         <v>0.5</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>24</v>
-      </c>
       <c r="D6" s="5">
-        <v>0.5</v>
+        <v>3</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D7" s="5">
         <v>3</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D8" s="5">
         <v>3</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D9" s="5">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="5">
+        <v>3</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="5" t="s">
+      <c r="B11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="5">
-        <v>6</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
+      <c r="D11" s="5">
+        <v>5</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="5" t="s">
+      <c r="B12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>35</v>
-      </c>
-      <c r="D11" s="5">
-        <v>3</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>38</v>
       </c>
       <c r="D12" s="5">
         <v>5</v>
@@ -865,256 +847,258 @@
         <v>9</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="5">
+        <v>8</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B14" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="5">
+        <v>2</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D13" s="5">
-        <v>5</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C14" s="5" t="s">
+      <c r="C15" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="D14" s="5">
-        <v>8</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
+      <c r="D15" s="5">
+        <v>1</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" s="5" t="s">
         <v>43</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="D15" s="5">
-        <v>2</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>46</v>
-      </c>
       <c r="D16" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17" s="5">
+        <v>2</v>
+      </c>
+      <c r="E17" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D17" s="5"/>
-      <c r="E17" s="3" t="s">
-        <v>9</v>
-      </c>
       <c r="F17" s="5" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="5" t="s">
         <v>50</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>51</v>
       </c>
       <c r="D18" s="5">
         <v>2</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>36</v>
+        <v>9</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C19" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D19" s="5">
+        <v>1</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
         <v>53</v>
-      </c>
-      <c r="D19" s="5">
-        <v>2</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="4" t="s">
-        <v>54</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D20" s="5">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>9</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B21" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>57</v>
-      </c>
       <c r="D21" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>9</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B22" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C22" s="5" t="s">
+      <c r="D22" s="5">
+        <v>2</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="D22" s="5">
+      <c r="B23" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D23" s="5">
+        <v>1</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D24" s="5">
         <v>4</v>
       </c>
-      <c r="E22" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A23" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="D23" s="5">
-        <v>3</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F23" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A24" s="4" t="s">
+      <c r="E24" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A25" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B24" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C24" s="5" t="s">
+      <c r="B25" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C25" s="5" t="s">
         <v>64</v>
-      </c>
-      <c r="D24" s="5">
-        <v>2</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F24" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>66</v>
       </c>
       <c r="D25" s="5">
         <v>1</v>
@@ -1123,67 +1107,27 @@
         <v>9</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D26" s="5">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>9</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A27" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="D27" s="5">
-        <v>1</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="F27" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A28" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="D28" s="5">
-        <v>2</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F28" s="5" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -1213,8 +1157,6 @@
     <hyperlink ref="A24" r:id="rId23"/>
     <hyperlink ref="A25" r:id="rId24"/>
     <hyperlink ref="A26" r:id="rId25"/>
-    <hyperlink ref="A27" r:id="rId26"/>
-    <hyperlink ref="A28" r:id="rId27"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>